<commit_message>
updated sprint 4 backlog
updated the sprint 4 backlog to include more detailed tasks to split up the issues and tasks to smaller peices

-Corey Williams
</commit_message>
<xml_diff>
--- a/sprints/sprint4/SprintBacklog/Sprint Backlog & BurndownSprint4.xlsx
+++ b/sprints/sprint4/SprintBacklog/Sprint Backlog & BurndownSprint4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhtpa\Desktop\Group3Spring2024Capstone\sprints\sprint4\SprintBacklog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8E3648-B4DF-4E97-A368-C49159BBDBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8BA6F0-C80B-48AD-A1C6-AC04BE883223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19095" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Related User Story</t>
   </si>
@@ -77,16 +77,46 @@
     <t>Fix Expanded Note Web Corey</t>
   </si>
   <si>
-    <t>Build Project Web Saul</t>
-  </si>
-  <si>
-    <t>Build Project Desktop Saul</t>
-  </si>
-  <si>
     <t>Export a list of sources Web Corey</t>
   </si>
   <si>
     <t>Export a list of sources Desktop Corey</t>
+  </si>
+  <si>
+    <t>create basic layout Project Page Web Saul</t>
+  </si>
+  <si>
+    <t>create basic layout Project Page Desktop Saul</t>
+  </si>
+  <si>
+    <t>implement add source project page web saul</t>
+  </si>
+  <si>
+    <t>implement add source project page desktop saul</t>
+  </si>
+  <si>
+    <t>implement remove source project page web saul</t>
+  </si>
+  <si>
+    <t>implement remove source project page desktop saul</t>
+  </si>
+  <si>
+    <t>create export list of sources dialog web corey</t>
+  </si>
+  <si>
+    <t>create export list of sources dialog desktop corey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implment the formated sources web corey </t>
+  </si>
+  <si>
+    <t xml:space="preserve">implment the formated sources desktop corey </t>
+  </si>
+  <si>
+    <t>update class diagram for web corey</t>
+  </si>
+  <si>
+    <t>fix sprint backlog 4 diagram corey</t>
   </si>
 </sst>
 </file>
@@ -292,46 +322,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>34.5</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -719,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -857,7 +887,7 @@
         <v>3</v>
       </c>
       <c r="Q3" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -905,10 +935,10 @@
         <v>3</v>
       </c>
       <c r="P4" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q4" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -917,49 +947,49 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N5" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O5" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P5" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q5" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -968,49 +998,49 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="3">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N6" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O6" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P6" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q6" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1019,49 +1049,49 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D7" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E7" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F7" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G7" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H7" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I7" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J7" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K7" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L7" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M7" s="3">
         <v>3</v>
       </c>
       <c r="N7" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O7" s="3">
         <v>3</v>
       </c>
       <c r="P7" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q7" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1070,49 +1100,49 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D8" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E8" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F8" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G8" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H8" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I8" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J8" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K8" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L8" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M8" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N8" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O8" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P8" s="3">
         <v>3</v>
       </c>
       <c r="Q8" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1121,49 +1151,49 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H9" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I9" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J9" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K9" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L9" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M9" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N9" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O9" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P9" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q9" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1172,49 +1202,49 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H10" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I10" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J10" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K10" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L10" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M10" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N10" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O10" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P10" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q10" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1223,49 +1253,49 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H11" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I11" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J11" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K11" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L11" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M11" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N11" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O11" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P11" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q11" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1273,211 +1303,561 @@
         <v>15</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3">
+        <v>3</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3</v>
+      </c>
+      <c r="I12" s="3">
+        <v>3</v>
+      </c>
+      <c r="J12" s="3">
+        <v>3</v>
+      </c>
+      <c r="K12" s="3">
+        <v>3</v>
+      </c>
+      <c r="L12" s="3">
+        <v>3</v>
+      </c>
+      <c r="M12" s="3">
+        <v>3</v>
+      </c>
+      <c r="N12" s="3">
+        <v>3</v>
+      </c>
+      <c r="O12" s="3">
+        <v>3</v>
+      </c>
+      <c r="P12" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
+      <c r="C13" s="2">
+        <v>3</v>
+      </c>
+      <c r="D13" s="3">
+        <v>3</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3">
+        <v>3</v>
+      </c>
+      <c r="G13" s="3">
+        <v>3</v>
+      </c>
+      <c r="H13" s="3">
+        <v>3</v>
+      </c>
+      <c r="I13" s="3">
+        <v>3</v>
+      </c>
+      <c r="J13" s="3">
+        <v>3</v>
+      </c>
+      <c r="K13" s="3">
+        <v>3</v>
+      </c>
+      <c r="L13" s="3">
+        <v>3</v>
+      </c>
+      <c r="M13" s="3">
+        <v>3</v>
+      </c>
+      <c r="N13" s="3">
+        <v>3</v>
+      </c>
+      <c r="O13" s="3">
+        <v>3</v>
+      </c>
+      <c r="P13" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
+      <c r="C14" s="2">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3</v>
+      </c>
+      <c r="H14" s="3">
+        <v>3</v>
+      </c>
+      <c r="I14" s="3">
+        <v>3</v>
+      </c>
+      <c r="J14" s="3">
+        <v>3</v>
+      </c>
+      <c r="K14" s="3">
+        <v>3</v>
+      </c>
+      <c r="L14" s="3">
+        <v>3</v>
+      </c>
+      <c r="M14" s="3">
+        <v>3</v>
+      </c>
+      <c r="N14" s="3">
+        <v>3</v>
+      </c>
+      <c r="O14" s="3">
+        <v>3</v>
+      </c>
+      <c r="P14" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
+      <c r="C15" s="2">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3">
+        <v>3</v>
+      </c>
+      <c r="F15" s="3">
+        <v>3</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3">
+        <v>3</v>
+      </c>
+      <c r="I15" s="3">
+        <v>3</v>
+      </c>
+      <c r="J15" s="3">
+        <v>3</v>
+      </c>
+      <c r="K15" s="3">
+        <v>3</v>
+      </c>
+      <c r="L15" s="3">
+        <v>3</v>
+      </c>
+      <c r="M15" s="3">
+        <v>3</v>
+      </c>
+      <c r="N15" s="3">
+        <v>3</v>
+      </c>
+      <c r="O15" s="3">
+        <v>3</v>
+      </c>
+      <c r="P15" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
+      <c r="C16" s="2">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3</v>
+      </c>
+      <c r="E16" s="3">
+        <v>3</v>
+      </c>
+      <c r="F16" s="3">
+        <v>3</v>
+      </c>
+      <c r="G16" s="3">
+        <v>3</v>
+      </c>
+      <c r="H16" s="3">
+        <v>3</v>
+      </c>
+      <c r="I16" s="3">
+        <v>3</v>
+      </c>
+      <c r="J16" s="3">
+        <v>3</v>
+      </c>
+      <c r="K16" s="3">
+        <v>3</v>
+      </c>
+      <c r="L16" s="3">
+        <v>3</v>
+      </c>
+      <c r="M16" s="3">
+        <v>3</v>
+      </c>
+      <c r="N16" s="3">
+        <v>3</v>
+      </c>
+      <c r="O16" s="3">
+        <v>3</v>
+      </c>
+      <c r="P16" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
+      <c r="C17" s="2">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3</v>
+      </c>
+      <c r="G17" s="3">
+        <v>3</v>
+      </c>
+      <c r="H17" s="3">
+        <v>3</v>
+      </c>
+      <c r="I17" s="3">
+        <v>3</v>
+      </c>
+      <c r="J17" s="3">
+        <v>3</v>
+      </c>
+      <c r="K17" s="3">
+        <v>3</v>
+      </c>
+      <c r="L17" s="3">
+        <v>3</v>
+      </c>
+      <c r="M17" s="3">
+        <v>3</v>
+      </c>
+      <c r="N17" s="3">
+        <v>3</v>
+      </c>
+      <c r="O17" s="3">
+        <v>3</v>
+      </c>
+      <c r="P17" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
+      <c r="C18" s="2">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3">
+        <v>3</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3</v>
+      </c>
+      <c r="H18" s="3">
+        <v>3</v>
+      </c>
+      <c r="I18" s="3">
+        <v>3</v>
+      </c>
+      <c r="J18" s="3">
+        <v>3</v>
+      </c>
+      <c r="K18" s="3">
+        <v>3</v>
+      </c>
+      <c r="L18" s="3">
+        <v>3</v>
+      </c>
+      <c r="M18" s="3">
+        <v>3</v>
+      </c>
+      <c r="N18" s="3">
+        <v>3</v>
+      </c>
+      <c r="O18" s="3">
+        <v>3</v>
+      </c>
+      <c r="P18" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
+      <c r="C19" s="2">
+        <v>3</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3">
+        <v>3</v>
+      </c>
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+      <c r="H19" s="3">
+        <v>3</v>
+      </c>
+      <c r="I19" s="3">
+        <v>3</v>
+      </c>
+      <c r="J19" s="3">
+        <v>3</v>
+      </c>
+      <c r="K19" s="3">
+        <v>3</v>
+      </c>
+      <c r="L19" s="3">
+        <v>3</v>
+      </c>
+      <c r="M19" s="3">
+        <v>3</v>
+      </c>
+      <c r="N19" s="3">
+        <v>3</v>
+      </c>
+      <c r="O19" s="3">
+        <v>3</v>
+      </c>
+      <c r="P19" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
+      <c r="C20" s="2">
+        <v>3</v>
+      </c>
+      <c r="D20" s="3">
+        <v>3</v>
+      </c>
+      <c r="E20" s="3">
+        <v>3</v>
+      </c>
+      <c r="F20" s="3">
+        <v>3</v>
+      </c>
+      <c r="G20" s="3">
+        <v>3</v>
+      </c>
+      <c r="H20" s="3">
+        <v>3</v>
+      </c>
+      <c r="I20" s="3">
+        <v>3</v>
+      </c>
+      <c r="J20" s="3">
+        <v>3</v>
+      </c>
+      <c r="K20" s="3">
+        <v>3</v>
+      </c>
+      <c r="L20" s="3">
+        <v>3</v>
+      </c>
+      <c r="M20" s="3">
+        <v>3</v>
+      </c>
+      <c r="N20" s="3">
+        <v>3</v>
+      </c>
+      <c r="O20" s="3">
+        <v>3</v>
+      </c>
+      <c r="P20" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3">
+        <v>2</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2</v>
+      </c>
+      <c r="H21" s="3">
+        <v>2</v>
+      </c>
+      <c r="I21" s="3">
+        <v>2</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0</v>
+      </c>
+      <c r="N21" s="3">
+        <v>0</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0</v>
+      </c>
+      <c r="P21" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3">
+        <v>1</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0</v>
+      </c>
+      <c r="N22" s="3">
+        <v>0</v>
+      </c>
+      <c r="O22" s="3">
+        <v>0</v>
+      </c>
+      <c r="P22" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
@@ -1561,63 +1941,63 @@
       </c>
       <c r="C27" s="5">
         <f t="shared" ref="C27:N27" si="0">SUM(C3:C26)</f>
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="D27" s="5">
         <f t="shared" si="0"/>
-        <v>34.5</v>
+        <v>57</v>
       </c>
       <c r="E27" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="G27" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="H27" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="I27" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="J27" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="K27" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="L27" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="M27" s="5">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="N27" s="5">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="O27" s="5">
         <f>SUM(O3:O26)</f>
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="P27" s="7">
         <f>SUM(P3:P26)</f>
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="Q27" s="7">
         <f>SUM(Q3:Q26)</f>
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed missing sprint 4 backlog
The sprint 4 backlog was missing and I recreated it so we have documentation for the procress made
</commit_message>
<xml_diff>
--- a/sprints/sprint4/SprintBacklog/Sprint Backlog & BurndownSprint4.xlsx
+++ b/sprints/sprint4/SprintBacklog/Sprint Backlog & BurndownSprint4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhtpa\Desktop\Group3Spring2024Capstone\sprints\sprint4\SprintBacklog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Captsone\Group3Spring2024Capstone\sprints\sprint4\SprintBacklog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8E3648-B4DF-4E97-A368-C49159BBDBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93D2E89-225A-4294-9EDC-C81D445836F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19095" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Related User Story</t>
   </si>
@@ -71,22 +71,40 @@
     <t>Update Noteviewer Web Saul</t>
   </si>
   <si>
-    <t>Fix Expanded Note Desktop Corey</t>
-  </si>
-  <si>
     <t>Fix Expanded Note Web Corey</t>
   </si>
   <si>
-    <t>Build Project Web Saul</t>
+    <t>Create Basic Project Page Layout Web Corey</t>
   </si>
   <si>
-    <t>Build Project Desktop Saul</t>
+    <t>Add and Delete Project Web Corey</t>
   </si>
   <si>
-    <t>Export a list of sources Web Corey</t>
+    <t>Create basic Project Viewer web Corey</t>
   </si>
   <si>
-    <t>Export a list of sources Desktop Corey</t>
+    <t>Add and Delete Source web Corey</t>
+  </si>
+  <si>
+    <t>export sources to BibTex format web Corey</t>
+  </si>
+  <si>
+    <t>Create Basic Project Page Layout Desktop saul</t>
+  </si>
+  <si>
+    <t>Add and Delete Project Desktop Saul</t>
+  </si>
+  <si>
+    <t>Create basic Project Viewer Desktop Saul</t>
+  </si>
+  <si>
+    <t>Add and Delete Source Desktop Saul</t>
+  </si>
+  <si>
+    <t>export sources to BibTex format Desktop Saul</t>
+  </si>
+  <si>
+    <t>Fix ASP Class Diagram Corey</t>
   </si>
 </sst>
 </file>
@@ -292,46 +310,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>34.5</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -719,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -857,7 +875,7 @@
         <v>3</v>
       </c>
       <c r="Q3" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -905,10 +923,10 @@
         <v>3</v>
       </c>
       <c r="P4" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q4" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -944,10 +962,10 @@
         <v>2</v>
       </c>
       <c r="L5" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M5" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N5" s="3">
         <v>0</v>
@@ -964,7 +982,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2">
@@ -1001,61 +1019,61 @@
         <v>2</v>
       </c>
       <c r="N6" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O6" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P6" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D7" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E7" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F7" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G7" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H7" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I7" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J7" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K7" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L7" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M7" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N7" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="O7" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P7" s="3">
         <v>0</v>
@@ -1066,50 +1084,50 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D8" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E8" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F8" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G8" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H8" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I8" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J8" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K8" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L8" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M8" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="N8" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O8" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P8" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="3">
         <v>0</v>
@@ -1121,46 +1139,46 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D9" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F9" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G9" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H9" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I9" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J9" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K9" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L9" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M9" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N9" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O9" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P9" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="3">
         <v>0</v>
@@ -1172,46 +1190,46 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D10" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E10" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G10" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H10" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I10" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J10" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K10" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L10" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M10" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N10" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O10" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P10" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="3">
         <v>0</v>
@@ -1223,46 +1241,46 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N11" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O11" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="3">
         <v>0</v>
@@ -1273,138 +1291,359 @@
         <v>15</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2</v>
+      </c>
+      <c r="J12" s="3">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3">
+        <v>2</v>
+      </c>
+      <c r="L12" s="3">
+        <v>2</v>
+      </c>
+      <c r="M12" s="3">
+        <v>2</v>
+      </c>
+      <c r="N12" s="3">
+        <v>2</v>
+      </c>
+      <c r="O12" s="3">
+        <v>2</v>
+      </c>
+      <c r="P12" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3">
+        <v>2</v>
+      </c>
+      <c r="I13" s="3">
+        <v>2</v>
+      </c>
+      <c r="J13" s="3">
+        <v>2</v>
+      </c>
+      <c r="K13" s="3">
+        <v>2</v>
+      </c>
+      <c r="L13" s="3">
+        <v>2</v>
+      </c>
+      <c r="M13" s="3">
+        <v>2</v>
+      </c>
+      <c r="N13" s="3">
+        <v>2</v>
+      </c>
+      <c r="O13" s="3">
+        <v>2</v>
+      </c>
+      <c r="P13" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3">
+        <v>2</v>
+      </c>
+      <c r="I14" s="3">
+        <v>2</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2</v>
+      </c>
+      <c r="K14" s="3">
+        <v>2</v>
+      </c>
+      <c r="L14" s="3">
+        <v>2</v>
+      </c>
+      <c r="M14" s="3">
+        <v>2</v>
+      </c>
+      <c r="N14" s="3">
+        <v>2</v>
+      </c>
+      <c r="O14" s="3">
+        <v>2</v>
+      </c>
+      <c r="P14" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3">
+        <v>2</v>
+      </c>
+      <c r="I15" s="3">
+        <v>2</v>
+      </c>
+      <c r="J15" s="3">
+        <v>2</v>
+      </c>
+      <c r="K15" s="3">
+        <v>2</v>
+      </c>
+      <c r="L15" s="3">
+        <v>2</v>
+      </c>
+      <c r="M15" s="3">
+        <v>2</v>
+      </c>
+      <c r="N15" s="3">
+        <v>2</v>
+      </c>
+      <c r="O15" s="3">
+        <v>2</v>
+      </c>
+      <c r="P15" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3">
+        <v>2</v>
+      </c>
+      <c r="I16" s="3">
+        <v>2</v>
+      </c>
+      <c r="J16" s="3">
+        <v>2</v>
+      </c>
+      <c r="K16" s="3">
+        <v>2</v>
+      </c>
+      <c r="L16" s="3">
+        <v>2</v>
+      </c>
+      <c r="M16" s="3">
+        <v>2</v>
+      </c>
+      <c r="N16" s="3">
+        <v>2</v>
+      </c>
+      <c r="O16" s="3">
+        <v>2</v>
+      </c>
+      <c r="P16" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>2</v>
+      </c>
+      <c r="F17" s="3">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3">
+        <v>2</v>
+      </c>
+      <c r="I17" s="3">
+        <v>2</v>
+      </c>
+      <c r="J17" s="3">
+        <v>2</v>
+      </c>
+      <c r="K17" s="3">
+        <v>2</v>
+      </c>
+      <c r="L17" s="3">
+        <v>2</v>
+      </c>
+      <c r="M17" s="3">
+        <v>2</v>
+      </c>
+      <c r="N17" s="3">
+        <v>2</v>
+      </c>
+      <c r="O17" s="3">
+        <v>2</v>
+      </c>
+      <c r="P17" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2</v>
+      </c>
+      <c r="H18" s="3">
+        <v>2</v>
+      </c>
+      <c r="I18" s="3">
+        <v>2</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+      <c r="N18" s="3">
+        <v>0</v>
+      </c>
+      <c r="O18" s="3">
+        <v>0</v>
+      </c>
+      <c r="P18" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
@@ -1561,63 +1800,63 @@
       </c>
       <c r="C27" s="5">
         <f t="shared" ref="C27:N27" si="0">SUM(C3:C26)</f>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D27" s="5">
         <f t="shared" si="0"/>
-        <v>34.5</v>
+        <v>33.5</v>
       </c>
       <c r="E27" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G27" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H27" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I27" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J27" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K27" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L27" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M27" s="5">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N27" s="5">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O27" s="5">
         <f>SUM(O3:O26)</f>
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="P27" s="7">
         <f>SUM(P3:P26)</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="Q27" s="7">
         <f>SUM(Q3:Q26)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>